<commit_message>
more project loading work, more cleaning
</commit_message>
<xml_diff>
--- a/Timekeeping/2024/03-24/LOTFI S 03-24.xlsx
+++ b/Timekeeping/2024/03-24/LOTFI S 03-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Timekeeping\03-24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\353-final-project\Timekeeping\2024\03-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD9FC37-2B51-4F49-B4AD-DE4468672274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1978C3-2808-401E-AA8C-4D410E4AA80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1485" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,9 +351,6 @@
     <t>Emery Phase 4</t>
   </si>
   <si>
-    <t>February 2024</t>
-  </si>
-  <si>
     <t>FEA</t>
   </si>
   <si>
@@ -388,6 +385,9 @@
   </si>
   <si>
     <t xml:space="preserve">Happy Hour </t>
+  </si>
+  <si>
+    <t>March 2024</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1329,8 @@
   </sheetPr>
   <dimension ref="A1:GH84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
       <c r="AH3" s="4"/>
       <c r="AI3" s="32"/>
       <c r="AJ3" s="75" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="AK3" s="30"/>
       <c r="AL3" s="30"/>
@@ -4533,7 +4533,7 @@
         <v>1</v>
       </c>
       <c r="AJ23" s="51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AK23" s="30"/>
       <c r="AL23" s="30"/>
@@ -4931,7 +4931,7 @@
         <v>3</v>
       </c>
       <c r="AJ25" s="51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AK25" s="30"/>
       <c r="AL25" s="30"/>
@@ -5558,10 +5558,10 @@
     </row>
     <row r="33" spans="1:52" s="30" customFormat="1" ht="10.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>106</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>107</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="65"/>
@@ -5625,7 +5625,7 @@
       </c>
       <c r="G34" s="65"/>
       <c r="H34" s="65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I34" s="65"/>
       <c r="J34" s="65"/>
@@ -5658,10 +5658,10 @@
     </row>
     <row r="35" spans="1:52" s="30" customFormat="1" ht="10" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>108</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>109</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="65"/>
@@ -5671,7 +5671,7 @@
       </c>
       <c r="G35" s="67"/>
       <c r="H35" s="67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I35" s="67"/>
       <c r="J35" s="65"/>
@@ -5714,7 +5714,7 @@
         <v>24</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="67"/>
@@ -5724,7 +5724,7 @@
       </c>
       <c r="G36" s="67"/>
       <c r="H36" s="67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I36" s="67"/>
       <c r="J36" s="67"/>
@@ -5759,13 +5759,13 @@
         <v>28</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="67"/>
       <c r="E37" s="67"/>
       <c r="F37" s="65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G37" s="65"/>
       <c r="H37" s="65" t="s">

</xml_diff>